<commit_message>
update of meta data and remove redundant files.
</commit_message>
<xml_diff>
--- a/src/main/resources/metadata.xlsx
+++ b/src/main/resources/metadata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="805"/>
@@ -2044,8 +2044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA554"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G282" workbookViewId="0">
-      <selection activeCell="Z316" sqref="Z1:Z1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H204" workbookViewId="0">
+      <selection activeCell="X221" sqref="X221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16506,7 +16506,7 @@
         <v>55</v>
       </c>
       <c r="X174" s="9" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="Y174" s="11" t="s">
         <v>432</v>
@@ -20324,7 +20324,7 @@
         <v>2</v>
       </c>
       <c r="X220" s="9" t="s">
-        <v>2</v>
+        <v>408</v>
       </c>
       <c r="Y220" s="11" t="s">
         <v>399</v>

</xml_diff>